<commit_message>
20190201 from my surface
</commit_message>
<xml_diff>
--- a/config/项目库.xlsx
+++ b/config/项目库.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16035" windowHeight="7860"/>
+    <workbookView windowWidth="19200" windowHeight="9070"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$32</definedName>
+  </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
   <si>
     <t>客户名称</t>
   </si>
@@ -45,12 +48,102 @@
     <t>备注</t>
   </si>
   <si>
+    <t>肖红</t>
+  </si>
+  <si>
+    <t>瑞龙制药尽职调查</t>
+  </si>
+  <si>
+    <t>瑞龙</t>
+  </si>
+  <si>
+    <t>扣差旅费：肖敏5665（王彬已付），王彬4390</t>
+  </si>
+  <si>
+    <t>周吉玲</t>
+  </si>
+  <si>
+    <t>周吉玲vs唐小军民间借贷纠纷</t>
+  </si>
+  <si>
+    <t>周吉</t>
+  </si>
+  <si>
+    <t>周</t>
+  </si>
+  <si>
+    <t>汇兴投资</t>
+  </si>
+  <si>
+    <t>法律顾问2017-2018</t>
+  </si>
+  <si>
+    <t>汇兴</t>
+  </si>
+  <si>
+    <t>顾问</t>
+  </si>
+  <si>
+    <t>郑彬</t>
+  </si>
+  <si>
+    <t>郑彬vs苍溪医院</t>
+  </si>
+  <si>
+    <t>扣罗烨希报差旅费1070</t>
+  </si>
+  <si>
+    <t>子腾医药</t>
+  </si>
+  <si>
+    <t>子腾|华奥|尚锐</t>
+  </si>
+  <si>
+    <t>瑞星行</t>
+  </si>
+  <si>
+    <t>瑞星行|瑞星公司</t>
+  </si>
+  <si>
+    <t>银河教育</t>
+  </si>
+  <si>
+    <t>银河</t>
+  </si>
+  <si>
+    <t>东区医院</t>
+  </si>
+  <si>
+    <t>法律顾问2018</t>
+  </si>
+  <si>
+    <t>东区;医院</t>
+  </si>
+  <si>
+    <t>绿满仓农业</t>
+  </si>
+  <si>
+    <t>绿满仓|绿华</t>
+  </si>
+  <si>
+    <t>农资集团</t>
+  </si>
+  <si>
+    <t>农资集团|川农资|农业生产|农业资料</t>
+  </si>
+  <si>
+    <t>每日经济新闻</t>
+  </si>
+  <si>
+    <t>法律顾问2018-2019上半年</t>
+  </si>
+  <si>
+    <t>每</t>
+  </si>
+  <si>
     <t>南环药业</t>
   </si>
   <si>
-    <t>法律顾问2017-2018</t>
-  </si>
-  <si>
     <t>南环</t>
   </si>
   <si>
@@ -66,18 +159,9 @@
     <t>顾|路</t>
   </si>
   <si>
-    <t>每日经济新闻</t>
-  </si>
-  <si>
     <t>法律顾问2017-2018下半年</t>
   </si>
   <si>
-    <t>每</t>
-  </si>
-  <si>
-    <t>顾问</t>
-  </si>
-  <si>
     <t>瑞星川物</t>
   </si>
   <si>
@@ -87,9 +171,6 @@
     <t>万欣</t>
   </si>
   <si>
-    <t>农资集团</t>
-  </si>
-  <si>
     <t>仲帮种业尽调</t>
   </si>
   <si>
@@ -102,15 +183,9 @@
     <t>派驻律师服务2017-2018</t>
   </si>
   <si>
-    <t>银河教育</t>
-  </si>
-  <si>
     <t>法律顾问2016-2017</t>
   </si>
   <si>
-    <t>银河</t>
-  </si>
-  <si>
     <t>金和矿业转让</t>
   </si>
   <si>
@@ -132,27 +207,9 @@
     <t>代持</t>
   </si>
   <si>
-    <t>瑞星行</t>
-  </si>
-  <si>
-    <t>瑞星行|瑞星公司</t>
-  </si>
-  <si>
-    <t>绿满仓农业</t>
-  </si>
-  <si>
     <t>法律顾问2017</t>
   </si>
   <si>
-    <t>绿满仓|绿华</t>
-  </si>
-  <si>
-    <t>农资集团|川农资|农业生产|农业资料</t>
-  </si>
-  <si>
-    <t>东区医院</t>
-  </si>
-  <si>
     <t>谭谷明vs东区医院人身权纠纷</t>
   </si>
   <si>
@@ -163,9 +220,6 @@
   </si>
   <si>
     <t>一审</t>
-  </si>
-  <si>
-    <t>东区;医院</t>
   </si>
   <si>
     <t>顶珍生物尽调</t>
@@ -249,7 +303,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,11 +324,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -293,7 +369,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,38 +393,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,6 +408,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -370,16 +423,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,6 +437,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -401,6 +455,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -413,7 +473,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,19 +521,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,13 +587,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,25 +599,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,91 +635,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,6 +646,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -606,15 +684,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,17 +703,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -653,7 +727,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -672,26 +746,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -700,10 +754,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -712,133 +766,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1174,15 +1228,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="23.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="33.75" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="6" width="11.5" customWidth="1"/>
@@ -1220,7 +1274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="1" spans="1:8">
+    <row r="2" customFormat="1" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1228,21 +1282,24 @@
         <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>42838</v>
+        <v>43229</v>
       </c>
       <c r="D2" s="1">
-        <v>43202</v>
+        <v>43385</v>
       </c>
       <c r="E2">
-        <v>10000</v>
+        <v>90000</v>
       </c>
       <c r="F2">
-        <v>10000</v>
+        <v>34945</v>
       </c>
       <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1251,253 +1308,262 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>42912</v>
+        <v>42656</v>
       </c>
       <c r="D3" s="1">
-        <v>43273</v>
+        <v>43452</v>
       </c>
       <c r="E3">
-        <v>30000</v>
+        <v>70000</v>
       </c>
       <c r="F3">
-        <v>15000</v>
+        <v>35000</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:8">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1">
-        <v>43082</v>
+        <v>42931</v>
       </c>
       <c r="D4" s="1">
-        <v>43263</v>
+        <v>43343</v>
       </c>
       <c r="E4">
-        <v>65000</v>
+        <v>60000</v>
       </c>
       <c r="F4">
-        <v>32500</v>
+        <v>30000</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" customFormat="1" spans="1:8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:9">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1">
-        <v>42879</v>
+        <v>43158</v>
       </c>
       <c r="D5" s="1">
-        <v>43243</v>
+        <v>43398</v>
       </c>
       <c r="E5">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="F5">
-        <v>20000</v>
+        <v>13930</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:8">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
-        <v>42826</v>
+        <v>43022</v>
       </c>
       <c r="D6" s="1">
-        <v>43190</v>
+        <v>43386</v>
       </c>
       <c r="E6">
-        <v>20000</v>
+        <v>100000</v>
       </c>
       <c r="F6">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:8">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
-        <v>42988</v>
+        <v>43022</v>
       </c>
       <c r="D7" s="1">
-        <v>43227</v>
+        <v>43386</v>
       </c>
       <c r="E7">
         <v>50000</v>
       </c>
       <c r="F7">
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" customFormat="1" spans="1:6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" spans="1:8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
-        <v>43070</v>
+        <v>43028</v>
       </c>
       <c r="D8" s="1">
-        <v>43434</v>
+        <v>43392</v>
       </c>
       <c r="E8">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="F8">
-        <v>100000</v>
+        <v>5000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:8">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
-        <v>42663</v>
+        <v>43101</v>
       </c>
       <c r="D9" s="1">
-        <v>43027</v>
+        <v>43465</v>
       </c>
       <c r="E9">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="F9">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:8">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="1">
-        <v>43057</v>
+        <v>43101</v>
       </c>
       <c r="D10" s="1">
-        <v>43166</v>
+        <v>43465</v>
       </c>
       <c r="E10">
-        <v>80000</v>
+        <v>30000</v>
       </c>
       <c r="F10">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="1:8">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1">
-        <v>43095</v>
+        <v>43101</v>
       </c>
       <c r="D11" s="1">
-        <v>43115</v>
+        <v>43465</v>
       </c>
       <c r="E11">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="F11">
-        <v>5000</v>
+        <v>25000</v>
       </c>
       <c r="G11" t="s">
         <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:8">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
       <c r="C12" s="1">
-        <v>42657</v>
+        <v>43264</v>
       </c>
       <c r="D12" s="1">
-        <v>43021</v>
+        <v>43446</v>
       </c>
       <c r="E12">
-        <v>50000</v>
+        <v>65000</v>
       </c>
       <c r="F12">
-        <v>25000</v>
+        <v>32500</v>
       </c>
       <c r="G12" t="s">
         <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:8">
@@ -1505,239 +1571,519 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42838</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43202</v>
+      </c>
+      <c r="E13">
+        <v>10000</v>
+      </c>
+      <c r="F13">
+        <v>10000</v>
+      </c>
+      <c r="G13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="1">
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" spans="1:8">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1">
+        <v>42912</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43273</v>
+      </c>
+      <c r="E14">
+        <v>30000</v>
+      </c>
+      <c r="F14">
+        <v>15000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:8">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43082</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43263</v>
+      </c>
+      <c r="E15">
+        <v>65000</v>
+      </c>
+      <c r="F15">
+        <v>32500</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" spans="1:8">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1">
+        <v>42879</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43243</v>
+      </c>
+      <c r="E16">
+        <v>40000</v>
+      </c>
+      <c r="F16">
+        <v>20000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:8">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1">
+        <v>42826</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43190</v>
+      </c>
+      <c r="E17">
+        <v>20000</v>
+      </c>
+      <c r="F17">
+        <v>20000</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" spans="1:8">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1">
+        <v>42988</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43227</v>
+      </c>
+      <c r="E18">
+        <v>50000</v>
+      </c>
+      <c r="F18">
+        <v>35000</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" spans="1:6">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43070</v>
+      </c>
+      <c r="D19" s="1">
+        <v>43434</v>
+      </c>
+      <c r="E19">
+        <v>69761</v>
+      </c>
+      <c r="F19">
+        <v>69761</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" spans="1:8">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42663</v>
+      </c>
+      <c r="D20" s="1">
+        <v>43027</v>
+      </c>
+      <c r="E20">
+        <v>10000</v>
+      </c>
+      <c r="F20">
+        <v>5000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" customFormat="1" spans="1:8">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43057</v>
+      </c>
+      <c r="D21" s="1">
+        <v>43166</v>
+      </c>
+      <c r="E21">
+        <v>80000</v>
+      </c>
+      <c r="F21">
+        <v>40000</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" customFormat="1" spans="1:8">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43095</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43115</v>
+      </c>
+      <c r="E22">
+        <v>5000</v>
+      </c>
+      <c r="F22">
+        <v>5000</v>
+      </c>
+      <c r="G22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" spans="1:8">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="1">
+        <v>42657</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43021</v>
+      </c>
+      <c r="E23">
+        <v>50000</v>
+      </c>
+      <c r="F23">
+        <v>25000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" spans="1:8">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1">
         <v>42736</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D24" s="1">
         <v>43100</v>
       </c>
-      <c r="E13">
+      <c r="E24">
         <v>30000</v>
       </c>
-      <c r="F13">
+      <c r="F24">
         <v>15000</v>
       </c>
-      <c r="G13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="1">
         <v>42736</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D25" s="1">
         <v>43100</v>
       </c>
-      <c r="E14">
+      <c r="E25">
         <v>50000</v>
       </c>
-      <c r="F14">
+      <c r="F25">
         <v>25000</v>
       </c>
-      <c r="G14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="G25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="1">
         <v>42922</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D26" s="1">
         <v>43312</v>
       </c>
-      <c r="E15">
+      <c r="E26">
         <v>20000</v>
       </c>
-      <c r="F15">
+      <c r="F26">
         <v>10000</v>
       </c>
-      <c r="G15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="G26" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="1">
         <v>42736</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D27" s="1">
         <v>43100</v>
       </c>
-      <c r="E16">
-        <v>3000</v>
-      </c>
-      <c r="F16">
+      <c r="E27">
+        <v>30000</v>
+      </c>
+      <c r="F27">
         <v>15000</v>
       </c>
-      <c r="G16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="1">
         <v>42983</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D28" s="1">
         <v>43019</v>
       </c>
-      <c r="E17">
+      <c r="E28">
         <v>50000</v>
       </c>
-      <c r="F17">
+      <c r="F28">
         <v>25000</v>
       </c>
-      <c r="G17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="G28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="H28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="1">
         <v>42824</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D29" s="1">
         <v>43161</v>
       </c>
-      <c r="E18">
+      <c r="E29">
         <v>36000</v>
       </c>
-      <c r="F18">
+      <c r="F29">
         <v>36000</v>
       </c>
-      <c r="G18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1">
         <v>42873</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D30" s="1">
         <v>43081</v>
       </c>
-      <c r="E19">
+      <c r="E30">
         <v>65000</v>
       </c>
-      <c r="F19">
+      <c r="F30">
         <v>32500</v>
       </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20">
+      <c r="G30" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31">
         <v>80000</v>
       </c>
-      <c r="F20">
+      <c r="F31">
         <v>40000</v>
       </c>
-      <c r="G20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21">
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32">
         <v>8000</v>
       </c>
-      <c r="F21">
+      <c r="F32">
         <v>4000</v>
       </c>
-      <c r="G21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" t="s">
-        <v>67</v>
+      <c r="G32" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +2101,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1771,7 +2117,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>